<commit_message>
Order History: minor typo fix
</commit_message>
<xml_diff>
--- a/asset/files/order-history.xlsx
+++ b/asset/files/order-history.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0E961816-357B-49FA-88BA-D9EA9CA474B6}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="637" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="637"/>
   </bookViews>
   <sheets>
     <sheet name="Legends" sheetId="11" r:id="rId1"/>
@@ -18,7 +17,7 @@
     <sheet name="7th order" sheetId="10" r:id="rId8"/>
     <sheet name="Budget" sheetId="5" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="159">
   <si>
     <t>Stock No.</t>
   </si>
@@ -343,9 +342,6 @@
   </si>
   <si>
     <t>Total Cost</t>
-  </si>
-  <si>
-    <t>Budger Left</t>
   </si>
   <si>
     <t>Budget Left</t>
@@ -513,13 +509,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
     <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
     <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.000"/>
     <numFmt numFmtId="165" formatCode="&quot;£&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -549,12 +545,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -816,45 +806,11 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -879,9 +835,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -899,7 +852,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -935,9 +887,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -950,13 +899,54 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1242,73 +1232,73 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37FE2BA9-1A61-42B1-B236-43F186877E37}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="39.20703125" customWidth="1"/>
+    <col min="2" max="2" width="39.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="B1" s="85" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="84" t="s">
+      <c r="B1" s="64" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="63" t="s">
+        <v>149</v>
+      </c>
+      <c r="B2" s="65"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="63" t="s">
         <v>150</v>
       </c>
-      <c r="B2" s="86"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="84" t="s">
+      <c r="B3" s="66"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="63" t="s">
         <v>151</v>
       </c>
-      <c r="B3" s="87"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="84" t="s">
+      <c r="B4" s="67"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="63" t="s">
         <v>152</v>
       </c>
-      <c r="B4" s="88"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="84" t="s">
+      <c r="B5" s="68"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="63" t="s">
         <v>153</v>
       </c>
-      <c r="B5" s="89"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="84" t="s">
+      <c r="B6" s="69"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="63" t="s">
         <v>154</v>
       </c>
-      <c r="B6" s="90"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="84" t="s">
+      <c r="B7" s="70"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="63" t="s">
         <v>155</v>
       </c>
-      <c r="B7" s="91"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="84" t="s">
+      <c r="B8" s="71"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="63" t="s">
         <v>156</v>
       </c>
-      <c r="B8" s="92"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="84" t="s">
-        <v>157</v>
-      </c>
-      <c r="B9" s="93"/>
+      <c r="B9" s="72"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1316,29 +1306,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView zoomScale="49" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.05078125" customWidth="1"/>
-    <col min="2" max="2" width="22.578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.3125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5234375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="10.68359375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.734375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="22.578125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="255.62890625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="22.5703125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="255.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="52" t="s">
-        <v>109</v>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="33" t="s">
+        <v>108</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>11</v>
@@ -1365,517 +1355,517 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="50" t="s">
-        <v>108</v>
-      </c>
-      <c r="B2" s="14" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="73" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" s="74" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="58" t="s">
-        <v>127</v>
-      </c>
-      <c r="D2" s="26">
+      <c r="C2" s="75" t="s">
+        <v>126</v>
+      </c>
+      <c r="D2" s="76">
         <v>11</v>
       </c>
-      <c r="E2" s="24">
+      <c r="E2" s="77">
         <v>13.18</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="78" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="24">
+      <c r="G2" s="77">
         <f>D2*E2</f>
         <v>144.97999999999999</v>
       </c>
-      <c r="H2" s="26" t="s">
-        <v>135</v>
-      </c>
-      <c r="I2" s="13" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="50" t="s">
-        <v>108</v>
-      </c>
-      <c r="B3" s="15" t="s">
+      <c r="H2" s="76" t="s">
+        <v>134</v>
+      </c>
+      <c r="I2" s="79" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="73" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="80" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="27">
-        <v>2</v>
-      </c>
-      <c r="E3" s="25">
+      <c r="D3" s="81">
+        <v>2</v>
+      </c>
+      <c r="E3" s="82">
         <v>0.55700000000000005</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="F3" s="83" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="25">
+      <c r="G3" s="82">
         <f t="shared" ref="G3:G18" si="0">D3*E3</f>
         <v>1.1140000000000001</v>
       </c>
-      <c r="H3" s="27" t="s">
+      <c r="H3" s="81" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="13" t="s">
+      <c r="I3" s="79" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="50" t="s">
-        <v>108</v>
-      </c>
-      <c r="B4" s="15" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="73" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="27">
-        <v>2</v>
-      </c>
-      <c r="E4" s="25">
+      <c r="D4" s="81">
+        <v>2</v>
+      </c>
+      <c r="E4" s="82">
         <v>0.55000000000000004</v>
       </c>
-      <c r="F4" s="23" t="s">
+      <c r="F4" s="83" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="25">
+      <c r="G4" s="82">
         <f t="shared" si="0"/>
         <v>1.1000000000000001</v>
       </c>
-      <c r="H4" s="27" t="s">
+      <c r="H4" s="81" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="13" t="s">
+      <c r="I4" s="79" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="50" t="s">
-        <v>108</v>
-      </c>
-      <c r="B5" s="15" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="73" t="s">
+        <v>107</v>
+      </c>
+      <c r="B5" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="84" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="27">
-        <v>2</v>
-      </c>
-      <c r="E5" s="25">
+      <c r="D5" s="81">
+        <v>2</v>
+      </c>
+      <c r="E5" s="82">
         <v>2.82</v>
       </c>
-      <c r="F5" s="23" t="s">
+      <c r="F5" s="83" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="25">
+      <c r="G5" s="82">
         <f t="shared" si="0"/>
         <v>5.64</v>
       </c>
-      <c r="H5" s="27" t="s">
+      <c r="H5" s="81" t="s">
         <v>18</v>
       </c>
-      <c r="I5" s="13" t="s">
+      <c r="I5" s="79" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="50" t="s">
-        <v>108</v>
-      </c>
-      <c r="B6" s="16" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="73" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="85" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="27">
-        <v>2</v>
-      </c>
-      <c r="E6" s="25">
-        <v>2</v>
-      </c>
-      <c r="F6" s="23">
+      <c r="D6" s="81">
+        <v>2</v>
+      </c>
+      <c r="E6" s="82">
+        <v>2</v>
+      </c>
+      <c r="F6" s="83">
         <v>5</v>
       </c>
-      <c r="G6" s="25">
+      <c r="G6" s="82">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="H6" s="27" t="s">
+      <c r="H6" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="I6" s="13" t="s">
+      <c r="I6" s="79" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="50" t="s">
-        <v>108</v>
-      </c>
-      <c r="B7" s="16" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="73" t="s">
+        <v>107</v>
+      </c>
+      <c r="B7" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="85" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="27">
-        <v>2</v>
-      </c>
-      <c r="E7" s="25">
+      <c r="D7" s="81">
+        <v>2</v>
+      </c>
+      <c r="E7" s="82">
         <v>2.2999999999999998</v>
       </c>
-      <c r="F7" s="23">
+      <c r="F7" s="83">
         <v>5</v>
       </c>
-      <c r="G7" s="25">
+      <c r="G7" s="82">
         <f t="shared" si="0"/>
         <v>4.5999999999999996</v>
       </c>
-      <c r="H7" s="27" t="s">
+      <c r="H7" s="81" t="s">
         <v>22</v>
       </c>
-      <c r="I7" s="13" t="s">
+      <c r="I7" s="79" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="50" t="s">
-        <v>108</v>
-      </c>
-      <c r="B8" s="15" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="73" t="s">
+        <v>107</v>
+      </c>
+      <c r="B8" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="84" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="27">
-        <v>2</v>
-      </c>
-      <c r="E8" s="25">
+      <c r="D8" s="81">
+        <v>2</v>
+      </c>
+      <c r="E8" s="82">
         <v>3.79</v>
       </c>
-      <c r="F8" s="23">
+      <c r="F8" s="83">
         <v>65</v>
       </c>
-      <c r="G8" s="25">
+      <c r="G8" s="82">
         <f t="shared" si="0"/>
         <v>7.58</v>
       </c>
-      <c r="H8" s="27" t="s">
+      <c r="H8" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="I8" s="13" t="s">
+      <c r="I8" s="79" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="50" t="s">
-        <v>108</v>
-      </c>
-      <c r="B9" s="15" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="73" t="s">
+        <v>107</v>
+      </c>
+      <c r="B9" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="84" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="27">
-        <v>2</v>
-      </c>
-      <c r="E9" s="25">
+      <c r="D9" s="81">
+        <v>2</v>
+      </c>
+      <c r="E9" s="82">
         <v>4.43</v>
       </c>
-      <c r="F9" s="23">
+      <c r="F9" s="83">
         <v>140</v>
       </c>
-      <c r="G9" s="25">
+      <c r="G9" s="82">
         <f t="shared" si="0"/>
         <v>8.86</v>
       </c>
-      <c r="H9" s="27" t="s">
+      <c r="H9" s="81" t="s">
         <v>34</v>
       </c>
-      <c r="I9" s="13" t="s">
+      <c r="I9" s="79" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="50" t="s">
-        <v>108</v>
-      </c>
-      <c r="B10" s="15" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="73" t="s">
+        <v>107</v>
+      </c>
+      <c r="B10" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="86" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="27">
-        <v>2</v>
-      </c>
-      <c r="E10" s="25">
+      <c r="D10" s="81">
+        <v>2</v>
+      </c>
+      <c r="E10" s="82">
         <v>0.57899999999999996</v>
       </c>
-      <c r="F10" s="23" t="s">
+      <c r="F10" s="83" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="25">
+      <c r="G10" s="82">
         <f t="shared" si="0"/>
         <v>1.1579999999999999</v>
       </c>
-      <c r="H10" s="27">
+      <c r="H10" s="81">
         <v>2056627</v>
       </c>
-      <c r="I10" s="13" t="s">
+      <c r="I10" s="79" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="50" t="s">
-        <v>108</v>
-      </c>
-      <c r="B11" s="15" t="s">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="73" t="s">
+        <v>107</v>
+      </c>
+      <c r="B11" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="85" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="27">
-        <v>2</v>
-      </c>
-      <c r="E11" s="25">
+      <c r="D11" s="81">
+        <v>2</v>
+      </c>
+      <c r="E11" s="82">
         <v>10.91</v>
       </c>
-      <c r="F11" s="23" t="s">
+      <c r="F11" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="G11" s="25">
+      <c r="G11" s="82">
         <f t="shared" si="0"/>
         <v>21.82</v>
       </c>
-      <c r="H11" s="27" t="s">
+      <c r="H11" s="81" t="s">
         <v>40</v>
       </c>
-      <c r="I11" s="13" t="s">
+      <c r="I11" s="79" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="50" t="s">
-        <v>108</v>
-      </c>
-      <c r="B12" s="15" t="s">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="73" t="s">
+        <v>107</v>
+      </c>
+      <c r="B12" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="85" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="27">
-        <v>2</v>
-      </c>
-      <c r="E12" s="25">
+      <c r="D12" s="81">
+        <v>2</v>
+      </c>
+      <c r="E12" s="82">
         <v>5.39</v>
       </c>
-      <c r="F12" s="23" t="s">
+      <c r="F12" s="83" t="s">
         <v>17</v>
       </c>
-      <c r="G12" s="25">
+      <c r="G12" s="82">
         <f t="shared" si="0"/>
         <v>10.78</v>
       </c>
-      <c r="H12" s="27" t="s">
+      <c r="H12" s="81" t="s">
         <v>41</v>
       </c>
-      <c r="I12" s="13" t="s">
+      <c r="I12" s="79" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="50" t="s">
-        <v>108</v>
-      </c>
-      <c r="B13" s="15" t="s">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="73" t="s">
+        <v>107</v>
+      </c>
+      <c r="B13" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="85" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="27">
-        <v>2</v>
-      </c>
-      <c r="E13" s="25">
+      <c r="D13" s="81">
+        <v>2</v>
+      </c>
+      <c r="E13" s="82">
         <v>4.97</v>
       </c>
-      <c r="F13" s="23">
+      <c r="F13" s="83">
         <v>50</v>
       </c>
-      <c r="G13" s="25">
+      <c r="G13" s="82">
         <f t="shared" si="0"/>
         <v>9.94</v>
       </c>
-      <c r="H13" s="27" t="s">
+      <c r="H13" s="81" t="s">
         <v>42</v>
       </c>
-      <c r="I13" s="13" t="s">
+      <c r="I13" s="79" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="51" t="s">
-        <v>108</v>
-      </c>
-      <c r="B14" s="15" t="s">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="73" t="s">
+        <v>107</v>
+      </c>
+      <c r="B14" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="C14" s="21" t="s">
+      <c r="C14" s="87" t="s">
         <v>54</v>
       </c>
-      <c r="D14" s="27">
-        <v>2</v>
-      </c>
-      <c r="E14" s="25">
+      <c r="D14" s="81">
+        <v>2</v>
+      </c>
+      <c r="E14" s="82">
         <v>0.03</v>
       </c>
-      <c r="F14" s="23" t="s">
+      <c r="F14" s="83" t="s">
         <v>17</v>
       </c>
-      <c r="G14" s="25">
+      <c r="G14" s="82">
         <f t="shared" si="0"/>
         <v>0.06</v>
       </c>
-      <c r="H14" s="27" t="s">
+      <c r="H14" s="81" t="s">
         <v>43</v>
       </c>
-      <c r="I14" s="13" t="s">
+      <c r="I14" s="79" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="51" t="s">
-        <v>108</v>
-      </c>
-      <c r="B15" s="15" t="s">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="73" t="s">
+        <v>107</v>
+      </c>
+      <c r="B15" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="C15" s="21" t="s">
+      <c r="C15" s="87" t="s">
         <v>55</v>
       </c>
-      <c r="D15" s="27">
-        <v>2</v>
-      </c>
-      <c r="E15" s="25">
+      <c r="D15" s="81">
+        <v>2</v>
+      </c>
+      <c r="E15" s="82">
         <v>0.04</v>
       </c>
-      <c r="F15" s="23" t="s">
+      <c r="F15" s="83" t="s">
         <v>17</v>
       </c>
-      <c r="G15" s="25">
+      <c r="G15" s="82">
         <f t="shared" si="0"/>
         <v>0.08</v>
       </c>
-      <c r="H15" s="27" t="s">
+      <c r="H15" s="81" t="s">
         <v>44</v>
       </c>
-      <c r="I15" s="13" t="s">
+      <c r="I15" s="79" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="51" t="s">
-        <v>108</v>
-      </c>
-      <c r="B16" s="15" t="s">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="73" t="s">
+        <v>107</v>
+      </c>
+      <c r="B16" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="85" t="s">
         <v>71</v>
       </c>
-      <c r="D16" s="27">
+      <c r="D16" s="81">
         <v>1</v>
       </c>
-      <c r="E16" s="25">
+      <c r="E16" s="82">
         <v>3.23</v>
       </c>
-      <c r="F16" s="23">
+      <c r="F16" s="83">
         <v>10</v>
       </c>
-      <c r="G16" s="25">
+      <c r="G16" s="82">
         <f t="shared" si="0"/>
         <v>3.23</v>
       </c>
-      <c r="H16" s="27" t="s">
+      <c r="H16" s="81" t="s">
         <v>72</v>
       </c>
-      <c r="I16" s="13" t="s">
+      <c r="I16" s="79" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="51" t="s">
-        <v>108</v>
-      </c>
-      <c r="B17" s="15" t="s">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="73" t="s">
+        <v>107</v>
+      </c>
+      <c r="B17" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="85" t="s">
         <v>73</v>
       </c>
-      <c r="D17" s="27">
+      <c r="D17" s="81">
         <v>1</v>
       </c>
-      <c r="E17" s="25">
+      <c r="E17" s="82">
         <v>1.22</v>
       </c>
-      <c r="F17" s="23">
+      <c r="F17" s="83">
         <v>20</v>
       </c>
-      <c r="G17" s="25">
+      <c r="G17" s="82">
         <f t="shared" si="0"/>
         <v>1.22</v>
       </c>
-      <c r="H17" s="27" t="s">
+      <c r="H17" s="81" t="s">
         <v>74</v>
       </c>
-      <c r="I17" s="13" t="s">
+      <c r="I17" s="79" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="51" t="s">
-        <v>108</v>
-      </c>
-      <c r="B18" s="28" t="s">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="73" t="s">
+        <v>107</v>
+      </c>
+      <c r="B18" s="88" t="s">
         <v>70</v>
       </c>
-      <c r="C18" s="29" t="s">
+      <c r="C18" s="89" t="s">
         <v>75</v>
       </c>
-      <c r="D18" s="32">
+      <c r="D18" s="90">
         <v>1</v>
       </c>
-      <c r="E18" s="31">
+      <c r="E18" s="91">
         <v>4.8499999999999996</v>
       </c>
-      <c r="F18" s="30">
+      <c r="F18" s="92">
         <v>50</v>
       </c>
-      <c r="G18" s="31">
+      <c r="G18" s="91">
         <f t="shared" si="0"/>
         <v>4.8499999999999996</v>
       </c>
-      <c r="H18" s="32" t="s">
+      <c r="H18" s="90" t="s">
         <v>76</v>
       </c>
-      <c r="I18" s="33" t="s">
+      <c r="I18" s="93" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F20" s="1" t="s">
         <v>77</v>
       </c>
@@ -1886,23 +1876,23 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="I4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="I8" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="I5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="I6" r:id="rId5" display="https://uk.rs-online.com/web/p/jack-trs-connectors/8104591/?searchTerm=810-4591&amp;relevancy-data=636F3D3126696E3D4931384E525353746F636B4E756D626572266C753D656E266D6D3D6D61746368616C6C26706D3D5E285C647B362C377D5B4161426250705D297C285C647B337D5B5C732D2F255C2E2C5D5C647B332C347D5B4161426250705D3F292426706F3D3126736E3D592673743D52535F53544F434B5F4E554D4245522677633D4E4F4E45267573743D3831302D34353931267374613D3831303435393126" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="I7" r:id="rId6" display="https://uk.rs-online.com/web/p/jack-trs-connectors/8104605/?searchTerm=810-4605&amp;relevancy-data=636F3D3126696E3D4931384E525353746F636B4E756D626572266C753D656E266D6D3D6D61746368616C6C26706D3D5E285C647B362C377D5B4161426250705D297C285C647B337D5B5C732D2F255C2E2C5D5C647B332C347D5B4161426250705D3F292426706F3D3126736E3D592673743D52535F53544F434B5F4E554D4245522677633D4E4F4E45267573743D3831302D34363035267374613D3831303436303526" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="I9" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="I10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="I12" r:id="rId9" display="https://uk.rs-online.com/web/p/centre-and-pin-punches/0733744/?searchTerm=733-744&amp;relevancy-data=636F3D3126696E3D4931384E525353746F636B4E756D626572266C753D656E266D6D3D6D61746368616C6C26706D3D5E285C647B362C377D5B4161426250705D297C285C647B337D5B5C732D2F255C2E2C5D5C647B332C347D5B4161426250705D3F292426706F3D3126736E3D592673743D52535F53544F434B5F4E554D4245522677633D4E4F4E45267573743D3733332D373434267374613D3037333337343426" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="I11" r:id="rId10" display="https://uk.rs-online.com/web/p/cable-sleeves/0408215/?searchTerm=408-215&amp;relevancy-data=636F3D3126696E3D4931384E525353746F636B4E756D626572266C753D656E266D6D3D6D61746368616C6C26706D3D5E285C647B362C377D5B4161426250705D297C285C647B337D5B5C732D2F255C2E2C5D5C647B332C347D5B4161426250705D3F292426706F3D3126736E3D592673743D52535F53544F434B5F4E554D4245522677633D4E4F4E45267573743D3430382D323135267374613D3034303832313526" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="I13" r:id="rId11" display="https://uk.rs-online.com/web/p/cable-tie-mounts/8111723/?searchTerm=811-1723&amp;relevancy-data=636F3D3126696E3D4931384E525353746F636B4E756D626572266C753D656E266D6D3D6D61746368616C6C26706D3D5E285C647B362C377D5B4161426250705D297C285C647B337D5B5C732D2F255C2E2C5D5C647B332C347D5B4161426250705D3F292426706F3D3126736E3D592673743D52535F53544F434B5F4E554D4245522677633D4E4F4E45267573743D3831312D31373233267374613D3831313137323326" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="I15" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="I14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="I16" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="I17" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="I18" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="I2" r:id="rId17" xr:uid="{E904722C-6359-40DD-9FC9-1D68A999E3F1}"/>
+    <hyperlink ref="I3" r:id="rId1"/>
+    <hyperlink ref="I4" r:id="rId2"/>
+    <hyperlink ref="I8" r:id="rId3"/>
+    <hyperlink ref="I5" r:id="rId4"/>
+    <hyperlink ref="I6" r:id="rId5" display="https://uk.rs-online.com/web/p/jack-trs-connectors/8104591/?searchTerm=810-4591&amp;relevancy-data=636F3D3126696E3D4931384E525353746F636B4E756D626572266C753D656E266D6D3D6D61746368616C6C26706D3D5E285C647B362C377D5B4161426250705D297C285C647B337D5B5C732D2F255C2E2C5D5C647B332C347D5B4161426250705D3F292426706F3D3126736E3D592673743D52535F53544F434B5F4E554D4245522677633D4E4F4E45267573743D3831302D34353931267374613D3831303435393126"/>
+    <hyperlink ref="I7" r:id="rId6" display="https://uk.rs-online.com/web/p/jack-trs-connectors/8104605/?searchTerm=810-4605&amp;relevancy-data=636F3D3126696E3D4931384E525353746F636B4E756D626572266C753D656E266D6D3D6D61746368616C6C26706D3D5E285C647B362C377D5B4161426250705D297C285C647B337D5B5C732D2F255C2E2C5D5C647B332C347D5B4161426250705D3F292426706F3D3126736E3D592673743D52535F53544F434B5F4E554D4245522677633D4E4F4E45267573743D3831302D34363035267374613D3831303436303526"/>
+    <hyperlink ref="I9" r:id="rId7"/>
+    <hyperlink ref="I10" r:id="rId8"/>
+    <hyperlink ref="I12" r:id="rId9" display="https://uk.rs-online.com/web/p/centre-and-pin-punches/0733744/?searchTerm=733-744&amp;relevancy-data=636F3D3126696E3D4931384E525353746F636B4E756D626572266C753D656E266D6D3D6D61746368616C6C26706D3D5E285C647B362C377D5B4161426250705D297C285C647B337D5B5C732D2F255C2E2C5D5C647B332C347D5B4161426250705D3F292426706F3D3126736E3D592673743D52535F53544F434B5F4E554D4245522677633D4E4F4E45267573743D3733332D373434267374613D3037333337343426"/>
+    <hyperlink ref="I11" r:id="rId10" display="https://uk.rs-online.com/web/p/cable-sleeves/0408215/?searchTerm=408-215&amp;relevancy-data=636F3D3126696E3D4931384E525353746F636B4E756D626572266C753D656E266D6D3D6D61746368616C6C26706D3D5E285C647B362C377D5B4161426250705D297C285C647B337D5B5C732D2F255C2E2C5D5C647B332C347D5B4161426250705D3F292426706F3D3126736E3D592673743D52535F53544F434B5F4E554D4245522677633D4E4F4E45267573743D3430382D323135267374613D3034303832313526"/>
+    <hyperlink ref="I13" r:id="rId11" display="https://uk.rs-online.com/web/p/cable-tie-mounts/8111723/?searchTerm=811-1723&amp;relevancy-data=636F3D3126696E3D4931384E525353746F636B4E756D626572266C753D656E266D6D3D6D61746368616C6C26706D3D5E285C647B362C377D5B4161426250705D297C285C647B337D5B5C732D2F255C2E2C5D5C647B332C347D5B4161426250705D3F292426706F3D3126736E3D592673743D52535F53544F434B5F4E554D4245522677633D4E4F4E45267573743D3831312D31373233267374613D3831313137323326"/>
+    <hyperlink ref="I15" r:id="rId12"/>
+    <hyperlink ref="I14" r:id="rId13"/>
+    <hyperlink ref="I16" r:id="rId14"/>
+    <hyperlink ref="I17" r:id="rId15"/>
+    <hyperlink ref="I18" r:id="rId16"/>
+    <hyperlink ref="I2" r:id="rId17"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId18"/>
@@ -1910,28 +1900,28 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView zoomScale="72" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.89453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="72.83984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.3125" customWidth="1"/>
-    <col min="5" max="5" width="11.83984375" customWidth="1"/>
-    <col min="6" max="6" width="10.734375" customWidth="1"/>
-    <col min="7" max="7" width="10.3671875" customWidth="1"/>
-    <col min="8" max="8" width="10.89453125" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="72.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" customWidth="1"/>
     <col min="9" max="9" width="99" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="52" t="s">
-        <v>109</v>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="33" t="s">
+        <v>108</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>11</v>
@@ -1958,127 +1948,127 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="51" t="s">
-        <v>108</v>
-      </c>
-      <c r="B2" s="34" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="D2" s="82">
+      <c r="D2" s="61">
         <v>1</v>
       </c>
-      <c r="E2" s="37">
+      <c r="E2" s="19">
         <v>2.09</v>
       </c>
-      <c r="F2" s="34">
+      <c r="F2" s="16">
         <v>50</v>
       </c>
-      <c r="G2" s="37">
+      <c r="G2" s="19">
         <f>D2*E2</f>
         <v>2.09</v>
       </c>
-      <c r="H2" s="34">
+      <c r="H2" s="16">
         <v>1419943</v>
       </c>
-      <c r="I2" s="35" t="s">
+      <c r="I2" s="17" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="51" t="s">
-        <v>108</v>
-      </c>
-      <c r="B3" s="34" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="D3" s="82">
+      <c r="D3" s="61">
         <v>1</v>
       </c>
-      <c r="E3" s="37">
+      <c r="E3" s="19">
         <v>3.46</v>
       </c>
-      <c r="F3" s="34">
+      <c r="F3" s="16">
         <v>50</v>
       </c>
-      <c r="G3" s="37">
+      <c r="G3" s="19">
         <f t="shared" ref="G3:G5" si="0">D3*E3</f>
         <v>3.46</v>
       </c>
-      <c r="H3" s="34">
+      <c r="H3" s="16">
         <v>1419945</v>
       </c>
-      <c r="I3" s="35" t="s">
+      <c r="I3" s="17" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="51" t="s">
-        <v>108</v>
-      </c>
-      <c r="B4" s="34" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="D4" s="82">
+      <c r="D4" s="61">
         <v>1</v>
       </c>
-      <c r="E4" s="37">
+      <c r="E4" s="19">
         <v>2.86</v>
       </c>
-      <c r="F4" s="34">
+      <c r="F4" s="16">
         <v>50</v>
       </c>
-      <c r="G4" s="37">
+      <c r="G4" s="19">
         <f t="shared" si="0"/>
         <v>2.86</v>
       </c>
-      <c r="H4" s="34">
+      <c r="H4" s="16">
         <v>1419946</v>
       </c>
-      <c r="I4" s="35" t="s">
+      <c r="I4" s="17" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="51" t="s">
-        <v>108</v>
-      </c>
-      <c r="B5" s="34" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="B5" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="D5" s="82">
+      <c r="D5" s="61">
         <v>1</v>
       </c>
-      <c r="E5" s="37">
+      <c r="E5" s="19">
         <v>4.29</v>
       </c>
-      <c r="F5" s="34">
+      <c r="F5" s="16">
         <v>50</v>
       </c>
-      <c r="G5" s="37">
+      <c r="G5" s="19">
         <f t="shared" si="0"/>
         <v>4.29</v>
       </c>
-      <c r="H5" s="34">
+      <c r="H5" s="16">
         <v>1419949</v>
       </c>
-      <c r="I5" s="35" t="s">
+      <c r="I5" s="17" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G7" s="12">
         <f>SUM(G2:G5)</f>
         <v>12.7</v>
@@ -2086,10 +2076,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I5" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="I2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="I3" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="I4" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="I5" r:id="rId1"/>
+    <hyperlink ref="I2" r:id="rId2"/>
+    <hyperlink ref="I3" r:id="rId3"/>
+    <hyperlink ref="I4" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
@@ -2097,300 +2087,300 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView zoomScale="92" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.41796875" customWidth="1"/>
-    <col min="2" max="2" width="19.9453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.68359375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.89453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="8.89453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.20703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.47265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="54.89453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="54.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="62" t="s">
-        <v>109</v>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="42" t="s">
+        <v>108</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="81" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="39" t="s">
+      <c r="D1" s="60" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="39" t="s">
+      <c r="F1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="39" t="s">
+      <c r="G1" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="39" t="s">
+      <c r="H1" s="21" t="s">
         <v>0</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="61" t="s">
-        <v>108</v>
-      </c>
-      <c r="B2" s="34" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="41" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="C2" s="43" t="s">
+      <c r="C2" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="D2" s="82">
-        <v>2</v>
-      </c>
-      <c r="E2" s="40">
+      <c r="D2" s="61">
+        <v>2</v>
+      </c>
+      <c r="E2" s="22">
         <v>12.76</v>
       </c>
-      <c r="F2" s="34">
+      <c r="F2" s="16">
         <v>1</v>
       </c>
-      <c r="G2" s="40">
+      <c r="G2" s="22">
         <f>D2*E2</f>
         <v>25.52</v>
       </c>
-      <c r="H2" s="41" t="s">
+      <c r="H2" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="I2" s="35" t="s">
+      <c r="I2" s="17" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="61" t="s">
-        <v>108</v>
-      </c>
-      <c r="B3" s="34" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="41" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="C3" s="44" t="s">
+      <c r="C3" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="D3" s="82">
-        <v>2</v>
-      </c>
-      <c r="E3" s="40">
+      <c r="D3" s="61">
+        <v>2</v>
+      </c>
+      <c r="E3" s="22">
         <v>6.33</v>
       </c>
-      <c r="F3" s="34">
+      <c r="F3" s="16">
         <v>1</v>
       </c>
-      <c r="G3" s="40">
+      <c r="G3" s="22">
         <f>D3*E3</f>
         <v>12.66</v>
       </c>
-      <c r="H3" s="41" t="s">
+      <c r="H3" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="I3" s="35" t="s">
+      <c r="I3" s="17" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="G5" s="42">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G5" s="24">
         <f>SUM(G2:G3)</f>
         <v>38.18</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="I3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="I2" r:id="rId1"/>
+    <hyperlink ref="I3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView zoomScale="73" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.3671875" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
     <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="83.5234375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.62890625" customWidth="1"/>
-    <col min="5" max="5" width="10.5234375" style="12" customWidth="1"/>
-    <col min="6" max="6" width="11.05078125" customWidth="1"/>
-    <col min="7" max="7" width="8.3671875" style="12" customWidth="1"/>
-    <col min="8" max="8" width="8.47265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="165.1015625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="83.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" style="12" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" style="12" customWidth="1"/>
+    <col min="8" max="8" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="165.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="62" t="s">
-        <v>109</v>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="42" t="s">
+        <v>108</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="39" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="53" t="s">
+      <c r="D1" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="39" t="s">
+      <c r="F1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="53" t="s">
+      <c r="G1" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="39" t="s">
+      <c r="H1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="71" t="s">
+      <c r="I1" s="51" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="60" t="s">
-        <v>108</v>
-      </c>
-      <c r="B2" s="65" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="40" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" s="45" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" s="47" t="s">
         <v>110</v>
       </c>
-      <c r="C2" s="67" t="s">
-        <v>111</v>
-      </c>
-      <c r="D2" s="79">
+      <c r="D2" s="58">
         <v>10</v>
       </c>
-      <c r="E2" s="69">
+      <c r="E2" s="49">
         <v>2.0099999999999998</v>
       </c>
-      <c r="F2" s="65">
+      <c r="F2" s="45">
         <v>1</v>
       </c>
-      <c r="G2" s="69">
+      <c r="G2" s="49">
         <f>D2*E2</f>
         <v>20.099999999999998</v>
       </c>
-      <c r="H2" s="65" t="s">
+      <c r="H2" s="45" t="s">
+        <v>111</v>
+      </c>
+      <c r="I2" s="43" t="s">
         <v>112</v>
       </c>
-      <c r="I2" s="63" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="60" t="s">
-        <v>108</v>
-      </c>
-      <c r="B3" s="65" t="s">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="40" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3" s="45" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3" s="47" t="s">
         <v>115</v>
       </c>
-      <c r="C3" s="67" t="s">
-        <v>116</v>
-      </c>
-      <c r="D3" s="79">
-        <v>2</v>
-      </c>
-      <c r="E3" s="69">
+      <c r="D3" s="58">
+        <v>2</v>
+      </c>
+      <c r="E3" s="49">
         <v>4.95</v>
       </c>
-      <c r="F3" s="65">
+      <c r="F3" s="45">
         <v>1</v>
       </c>
-      <c r="G3" s="69">
+      <c r="G3" s="49">
         <f>D3*E3</f>
         <v>9.9</v>
       </c>
-      <c r="H3" s="65" t="s">
+      <c r="H3" s="45" t="s">
+        <v>116</v>
+      </c>
+      <c r="I3" s="43" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="40" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" s="45" t="s">
+        <v>118</v>
+      </c>
+      <c r="C4" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="I3" s="63" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="60" t="s">
-        <v>108</v>
-      </c>
-      <c r="B4" s="65" t="s">
-        <v>119</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="D4" s="79">
-        <v>2</v>
-      </c>
-      <c r="E4" s="69">
+      <c r="D4" s="58">
+        <v>2</v>
+      </c>
+      <c r="E4" s="49">
         <v>2.2999999999999998</v>
       </c>
-      <c r="F4" s="65">
+      <c r="F4" s="45">
         <v>1</v>
       </c>
-      <c r="G4" s="69">
+      <c r="G4" s="49">
         <f>D4*E4</f>
         <v>4.5999999999999996</v>
       </c>
-      <c r="H4" s="65" t="s">
-        <v>121</v>
-      </c>
-      <c r="I4" s="63" t="s">
+      <c r="H4" s="45" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="61" t="s">
-        <v>108</v>
-      </c>
-      <c r="B5" s="66" t="s">
-        <v>124</v>
-      </c>
-      <c r="C5" s="68" t="s">
+      <c r="I4" s="43" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="41" t="s">
+        <v>107</v>
+      </c>
+      <c r="B5" s="46" t="s">
         <v>123</v>
       </c>
-      <c r="D5" s="80">
+      <c r="C5" s="48" t="s">
+        <v>122</v>
+      </c>
+      <c r="D5" s="59">
         <v>1</v>
       </c>
-      <c r="E5" s="70">
+      <c r="E5" s="50">
         <v>1.78</v>
       </c>
-      <c r="F5" s="66">
+      <c r="F5" s="46">
         <v>1</v>
       </c>
-      <c r="G5" s="70">
+      <c r="G5" s="50">
         <f>D5*E5</f>
         <v>1.78</v>
       </c>
-      <c r="H5" s="66">
+      <c r="H5" s="46">
         <v>1373965</v>
       </c>
-      <c r="I5" s="64" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="I5" s="44" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G7" s="12">
         <f>SUM(G2:G5)</f>
         <v>36.380000000000003</v>
@@ -2398,10 +2388,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-    <hyperlink ref="I4" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
-    <hyperlink ref="I3" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
-    <hyperlink ref="I5" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
+    <hyperlink ref="I2" r:id="rId1"/>
+    <hyperlink ref="I4" r:id="rId2"/>
+    <hyperlink ref="I3" r:id="rId3"/>
+    <hyperlink ref="I5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
@@ -2409,64 +2399,64 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53B7147A-D703-4F7E-854B-C549E464AA00}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.26171875" customWidth="1"/>
-    <col min="2" max="2" width="9.3125" customWidth="1"/>
-    <col min="3" max="3" width="55.83984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.83984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.20703125" customWidth="1"/>
-    <col min="6" max="6" width="9.9453125" customWidth="1"/>
-    <col min="7" max="7" width="8.734375" customWidth="1"/>
-    <col min="8" max="8" width="15.62890625" customWidth="1"/>
-    <col min="9" max="9" width="107.5234375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" customWidth="1"/>
+    <col min="3" max="3" width="55.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" customWidth="1"/>
+    <col min="9" max="9" width="107.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="52" t="s">
-        <v>109</v>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="33" t="s">
+        <v>108</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="39" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="53" t="s">
+      <c r="D1" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="39" t="s">
+      <c r="F1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="53" t="s">
+      <c r="G1" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="39" t="s">
+      <c r="H1" s="21" t="s">
         <v>0</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="51" t="s">
-        <v>108</v>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="32" t="s">
+        <v>107</v>
       </c>
       <c r="B2" t="s">
-        <v>131</v>
-      </c>
-      <c r="C2" s="54" t="s">
-        <v>129</v>
+        <v>130</v>
+      </c>
+      <c r="C2" s="35" t="s">
+        <v>128</v>
       </c>
       <c r="D2">
         <v>2</v>
@@ -2482,20 +2472,20 @@
         <v>14.62</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3" t="s">
         <v>132</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="51" t="s">
-        <v>108</v>
-      </c>
-      <c r="B3" t="s">
-        <v>133</v>
-      </c>
-      <c r="C3" s="54" t="s">
+      <c r="C3" s="35" t="s">
         <v>92</v>
       </c>
       <c r="D3">
@@ -2512,13 +2502,13 @@
         <v>26.5</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G5" s="12">
         <f>SUM(G2:G3)</f>
         <v>41.12</v>
@@ -2526,8 +2516,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" xr:uid="{077DDF28-4178-4D0B-8669-DE5106F59BD5}"/>
-    <hyperlink ref="I3" r:id="rId2" xr:uid="{6A04B296-35AF-42AA-A88B-68F84762423E}"/>
+    <hyperlink ref="I2" r:id="rId1"/>
+    <hyperlink ref="I3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -2535,149 +2525,148 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C64417C6-DAAC-4136-8916-03E3F2C0618B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.68359375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.83984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5234375" customWidth="1"/>
-    <col min="6" max="6" width="10.3671875" customWidth="1"/>
-    <col min="7" max="7" width="7.3671875" customWidth="1"/>
-    <col min="8" max="8" width="10.1015625" customWidth="1"/>
-    <col min="9" max="9" width="101.68359375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" customWidth="1"/>
+    <col min="7" max="7" width="7.42578125" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" customWidth="1"/>
+    <col min="9" max="9" width="101.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="62" t="s">
-        <v>109</v>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="42" t="s">
+        <v>108</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="39" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="53" t="s">
+      <c r="D1" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="39" t="s">
+      <c r="F1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="53" t="s">
+      <c r="G1" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="39" t="s">
+      <c r="H1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="71" t="s">
+      <c r="I1" s="51" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="60" t="s">
-        <v>108</v>
-      </c>
-      <c r="B2" s="65" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="40" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" s="45" t="s">
+        <v>114</v>
+      </c>
+      <c r="C2" s="47" t="s">
         <v>115</v>
       </c>
-      <c r="C2" s="67" t="s">
-        <v>116</v>
-      </c>
-      <c r="D2" s="79">
-        <v>2</v>
-      </c>
-      <c r="E2" s="69">
+      <c r="D2" s="58">
+        <v>2</v>
+      </c>
+      <c r="E2" s="49">
         <v>4.95</v>
       </c>
-      <c r="F2" s="65">
+      <c r="F2" s="45">
         <v>1</v>
       </c>
-      <c r="G2" s="69">
+      <c r="G2" s="49">
         <f>D2*E2</f>
         <v>9.9</v>
       </c>
-      <c r="H2" s="23" t="s">
-        <v>117</v>
-      </c>
-      <c r="I2" s="63" t="s">
-        <v>114</v>
+      <c r="H2" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="I2" s="43" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" xr:uid="{2DDEF242-78BB-457F-AA45-5953B31A6EAD}"/>
+    <hyperlink ref="I2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E8EF183-04BE-406D-9BAE-D63D6F3D0CA7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.3671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="63.47265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.15625" customWidth="1"/>
-    <col min="6" max="6" width="10.26171875" customWidth="1"/>
-    <col min="7" max="7" width="9.578125" customWidth="1"/>
-    <col min="8" max="8" width="9.5234375" customWidth="1"/>
-    <col min="9" max="9" width="153.5234375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" customWidth="1"/>
+    <col min="7" max="8" width="9.5703125" customWidth="1"/>
+    <col min="9" max="9" width="153.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="62" t="s">
-        <v>109</v>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="42" t="s">
+        <v>108</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="39" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="53" t="s">
+      <c r="D1" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="39" t="s">
+      <c r="F1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="53" t="s">
+      <c r="G1" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="39" t="s">
+      <c r="H1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="76" t="s">
+      <c r="I1" s="56" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="51" t="s">
-        <v>108</v>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="32" t="s">
+        <v>107</v>
       </c>
       <c r="B2" t="s">
-        <v>138</v>
-      </c>
-      <c r="C2" s="72" t="s">
+        <v>137</v>
+      </c>
+      <c r="C2" s="52" t="s">
         <v>90</v>
       </c>
       <c r="D2">
@@ -2700,14 +2689,14 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="51" t="s">
-        <v>108</v>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="32" t="s">
+        <v>107</v>
       </c>
       <c r="B3" t="s">
-        <v>139</v>
-      </c>
-      <c r="C3" s="72" t="s">
+        <v>138</v>
+      </c>
+      <c r="C3" s="52" t="s">
         <v>91</v>
       </c>
       <c r="D3">
@@ -2730,14 +2719,14 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="51" t="s">
-        <v>108</v>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="32" t="s">
+        <v>107</v>
       </c>
       <c r="B4" t="s">
-        <v>140</v>
-      </c>
-      <c r="C4" s="73" t="s">
+        <v>139</v>
+      </c>
+      <c r="C4" s="53" t="s">
         <v>62</v>
       </c>
       <c r="D4">
@@ -2760,15 +2749,15 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="51" t="s">
-        <v>108</v>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="32" t="s">
+        <v>107</v>
       </c>
       <c r="B5" t="s">
-        <v>141</v>
-      </c>
-      <c r="C5" s="83" t="s">
-        <v>143</v>
+        <v>140</v>
+      </c>
+      <c r="C5" s="62" t="s">
+        <v>142</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -2777,7 +2766,7 @@
         <v>8.9499999999999993</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G5" s="9">
         <f>D5*E5</f>
@@ -2790,15 +2779,15 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="74" t="s">
-        <v>108</v>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="54" t="s">
+        <v>107</v>
       </c>
       <c r="B6" t="s">
-        <v>147</v>
-      </c>
-      <c r="C6" s="54" t="s">
         <v>146</v>
+      </c>
+      <c r="C6" s="35" t="s">
+        <v>145</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -2813,28 +2802,28 @@
         <f>D6*E6</f>
         <v>5.54</v>
       </c>
-      <c r="H6" s="75" t="s">
+      <c r="H6" s="55" t="s">
+        <v>147</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="I6" s="2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G8" s="12">
         <f>SUM(G2:G6)</f>
         <v>71.590000000000018</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G10" s="12">
         <v>-7.22</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G11" s="12">
         <f>G8+G10</f>
         <v>64.370000000000019</v>
@@ -2842,11 +2831,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I3" r:id="rId1" xr:uid="{0663F069-3B51-4E4D-909C-AB7D989385C7}"/>
-    <hyperlink ref="I4" r:id="rId2" xr:uid="{6323F7D1-3434-41A4-9148-D854ECE5309A}"/>
-    <hyperlink ref="I2" r:id="rId3" xr:uid="{F6CE8695-CC81-4A7A-A7BD-BF3FD6677175}"/>
-    <hyperlink ref="I5" r:id="rId4" xr:uid="{3D6B2850-E3C4-4FCF-86E6-A751E667FE32}"/>
-    <hyperlink ref="I6" r:id="rId5" xr:uid="{C46193CE-C1E5-41EC-AA83-F5BA32912296}"/>
+    <hyperlink ref="I3" r:id="rId1"/>
+    <hyperlink ref="I4" r:id="rId2"/>
+    <hyperlink ref="I2" r:id="rId3"/>
+    <hyperlink ref="I5" r:id="rId4"/>
+    <hyperlink ref="I6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
@@ -2854,117 +2843,112 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:G12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.9453125" style="12"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="56" t="s">
-        <v>106</v>
-      </c>
-      <c r="C1" s="46">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="37" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" s="28">
         <v>500</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="56" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="37" t="s">
         <v>103</v>
       </c>
       <c r="B2" s="12">
         <v>231.012</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="56" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="37" t="s">
         <v>101</v>
       </c>
       <c r="B3" s="12">
         <v>12.7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="56" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="37" t="s">
         <v>102</v>
       </c>
-      <c r="B4" s="45">
+      <c r="B4" s="27">
         <v>38.18</v>
       </c>
-      <c r="C4" s="45"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="56" t="s">
-        <v>125</v>
-      </c>
-      <c r="B5" s="42">
+      <c r="C4" s="27"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="37" t="s">
+        <v>124</v>
+      </c>
+      <c r="B5" s="24">
         <v>36.380000000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="56" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="37" t="s">
+        <v>135</v>
+      </c>
+      <c r="B6" s="39">
+        <v>41.12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="37" t="s">
         <v>136</v>
       </c>
-      <c r="B6" s="59">
-        <v>41.12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="56" t="s">
-        <v>137</v>
-      </c>
-      <c r="B7" s="59">
+      <c r="B7" s="39">
         <v>9.9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="56" t="s">
-        <v>145</v>
-      </c>
-      <c r="B8" s="59">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="37" t="s">
+        <v>144</v>
+      </c>
+      <c r="B8" s="39">
         <v>64.37</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A9" s="57" t="s">
+    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="38" t="s">
         <v>104</v>
       </c>
-      <c r="B9" s="48" t="s">
-        <v>107</v>
-      </c>
-      <c r="C9" s="49">
+      <c r="B9" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" s="31">
         <f>SUM(B2:B8)</f>
         <v>433.66199999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="56" t="s">
+    <row r="10" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="37" t="s">
         <v>105</v>
       </c>
       <c r="B10" s="12"/>
-      <c r="C10" s="46">
+      <c r="C10" s="28">
         <f>500-C9</f>
         <v>66.338000000000022</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A11" s="78"/>
-      <c r="B11" s="48"/>
-      <c r="C11" s="49"/>
-      <c r="G11" s="55"/>
-    </row>
-    <row r="12" spans="1:7" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="77"/>
-      <c r="B12" s="45"/>
-      <c r="C12" s="47"/>
-      <c r="G12" s="55"/>
+      <c r="G10" s="36"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="57"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="29"/>
+      <c r="G11" s="36"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>